<commit_message>
trying to solve env and vscode problems added black formater and pylint
</commit_message>
<xml_diff>
--- a/Cチーム/開発演習_C.xlsx
+++ b/Cチーム/開発演習_C.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.200.200\共有f\01_講義資料\07_開発演習\Cチーム\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renerhoen/0-Dev/toshokan/Cチーム/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB49036F-1655-9649-AE80-DC9139F98C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26900" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBSガントチャート" sheetId="2" r:id="rId1"/>
@@ -19,10 +20,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">DBテーブル一覧表!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">変数一覧表!$A$1:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">関数一覧表!$A$1:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">変数一覧表!$A$1:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -132,22 +133,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="d\(aaa\)"/>
+    <numFmt numFmtId="164" formatCode="d\(aaa\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -392,10 +393,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
@@ -407,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
@@ -418,7 +419,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -445,46 +446,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル3" displayName="テーブル3" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="テーブル3" displayName="テーブル3" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No.">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No.">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="変数名"/>
-    <tableColumn id="3" name="モジュール名"/>
-    <tableColumn id="4" name="作成者"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="変数名"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="モジュール名"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="作成者"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="テーブル2" displayName="テーブル2" ref="A1:E2" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="No.">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="No.">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="関数名"/>
-    <tableColumn id="3" name="クラス名"/>
-    <tableColumn id="4" name="モジュール名"/>
-    <tableColumn id="5" name="作成者"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="関数名"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="クラス名"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="モジュール名"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="作成者"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="テーブル1" displayName="テーブル1" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No.">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="No.">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="テーブル名"/>
-    <tableColumn id="3" name="内容"/>
-    <tableColumn id="4" name="作成者"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="テーブル名"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="内容"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="作成者"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -752,20 +753,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="18" width="6.625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -821,7 +822,7 @@
         <v>44434</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -843,7 +844,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
       <c r="C3" s="6"/>
@@ -863,7 +864,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="6"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
       <c r="C4" s="6"/>
@@ -883,7 +884,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="1"/>
       <c r="C5" s="6"/>
@@ -903,7 +904,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="6"/>
@@ -923,7 +924,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="1"/>
       <c r="C7" s="6"/>
@@ -943,7 +944,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
@@ -963,7 +964,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
@@ -983,7 +984,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="1"/>
       <c r="C10" s="6"/>
@@ -1003,7 +1004,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="1"/>
       <c r="C11" s="6"/>
@@ -1023,7 +1024,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="1"/>
       <c r="C12" s="6"/>
@@ -1043,7 +1044,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="1"/>
       <c r="C13" s="6"/>
@@ -1063,7 +1064,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="1"/>
       <c r="C14" s="6"/>
@@ -1083,7 +1084,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="6"/>
@@ -1103,7 +1104,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="6"/>
@@ -1123,7 +1124,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="1"/>
       <c r="C17" s="6"/>
@@ -1143,7 +1144,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="6"/>
@@ -1163,7 +1164,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="6"/>
@@ -1183,7 +1184,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="1"/>
       <c r="C20" s="6"/>
@@ -1203,7 +1204,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="6"/>
@@ -1223,7 +1224,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="6"/>
@@ -1243,7 +1244,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="6"/>
@@ -1263,7 +1264,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
@@ -1285,7 +1286,7 @@
       <c r="Q24" s="16"/>
       <c r="R24" s="19"/>
     </row>
-    <row r="25" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>7</v>
       </c>
@@ -1319,22 +1320,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -1364,23 +1365,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -1413,22 +1414,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>

</xml_diff>